<commit_message>
Dalton min + graph of Jupiter act for mins
</commit_message>
<xml_diff>
--- a/Solar_consts.xlsx
+++ b/Solar_consts.xlsx
@@ -141,7 +141,7 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -162,7 +162,7 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -174,18 +174,213 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$B$3:$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Меркурий</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Венера</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Земля</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Марс</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Юпитер</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Сатурн</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Уран</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Нептун</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Плутон</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$H$3:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.35699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5569999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.73</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.036</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="59958400"/>
+        <c:axId val="59959936"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="59958400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="59959936"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="59959936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="59958400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1" title="Сила притяжения планет к Солнцу"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="B2:I12" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="B2:I12" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="B2:I12"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Объекты"/>
-    <tableColumn id="2" name="Масса, 10^24 кг" dataDxfId="7"/>
-    <tableColumn id="3" name="Удельная масса(Земля)" dataDxfId="6"/>
-    <tableColumn id="4" name="Радиус орбиты, усред., 10^9 м" dataDxfId="5"/>
-    <tableColumn id="5" name="Радиус орбиты  в радиусах Земли" dataDxfId="4"/>
-    <tableColumn id="6" name="Сила притяжения к Солнцу, 10^19 Н" dataDxfId="3"/>
-    <tableColumn id="7" name="Сила притяжения удельная, к Земле" dataDxfId="2"/>
-    <tableColumn id="8" name="Эксцентриситет" dataDxfId="1"/>
+    <tableColumn id="2" name="Масса, 10^24 кг" dataDxfId="6"/>
+    <tableColumn id="3" name="Удельная масса(Земля)" dataDxfId="5"/>
+    <tableColumn id="4" name="Радиус орбиты, усред., 10^9 м" dataDxfId="4"/>
+    <tableColumn id="5" name="Радиус орбиты  в радиусах Земли" dataDxfId="3"/>
+    <tableColumn id="6" name="Сила притяжения к Солнцу, 10^19 Н" dataDxfId="2"/>
+    <tableColumn id="7" name="Сила притяжения удельная, к Земле" dataDxfId="1"/>
+    <tableColumn id="8" name="Эксцентриситет" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -480,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,8 +1003,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>